<commit_message>
Termine la seccion de asignar perfiles
</commit_message>
<xml_diff>
--- a/Gestion de permisos.xlsx
+++ b/Gestion de permisos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\UAI\5- 1er Cuatrimestre 2024\Ingenieria de software\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD05584-D6BB-44A2-8A96-1366C5815F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014B92F5-ACB4-49E1-AFE6-1D58AF060C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AD3337A-49E2-40EF-8661-305EFD547F10}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AD3337A-49E2-40EF-8661-305EFD547F10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,13 +140,19 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -399,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -425,7 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,13 +444,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,6 +457,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9C73EA-1742-4FF6-8289-F6FEEBCE1BA8}">
   <dimension ref="B1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,20 +835,20 @@
       <c r="G2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="N2" s="19" t="s">
+      <c r="L2" s="23"/>
+      <c r="N2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="19"/>
+      <c r="O2" s="23"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -858,10 +866,10 @@
       <c r="G3" s="8">
         <v>1</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="4">
@@ -893,10 +901,10 @@
       <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="4">
@@ -928,10 +936,10 @@
       <c r="G5" s="4">
         <v>3</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="6">
@@ -966,7 +974,7 @@
       <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="O6" s="4">
@@ -995,7 +1003,7 @@
       <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>23</v>
       </c>
       <c r="N7" s="4">
@@ -1025,7 +1033,7 @@
       <c r="H8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>23</v>
       </c>
       <c r="N8" s="4">
@@ -1052,10 +1060,10 @@
       <c r="G9" s="4">
         <v>7</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="N9" s="4">
@@ -1081,10 +1089,10 @@
       <c r="G10" s="4">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1104,10 +1112,10 @@
       <c r="G11" s="4">
         <v>9</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1127,16 +1135,16 @@
       <c r="G12" s="4">
         <v>10</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="19" t="s">
+      <c r="I12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="19"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -1154,10 +1162,10 @@
       <c r="G13" s="4">
         <v>11</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="16" t="s">
         <v>22</v>
       </c>
       <c r="K13" s="4">
@@ -1183,10 +1191,10 @@
       <c r="G14" s="4">
         <v>12</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="K14" s="4">
@@ -1212,10 +1220,10 @@
       <c r="G15" s="4">
         <v>13</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1235,10 +1243,10 @@
       <c r="G16" s="4">
         <v>14</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1255,36 +1263,36 @@
       <c r="E17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="18">
         <v>15</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="20">
+      <c r="B18" s="18">
         <v>6</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="20">
-        <v>4</v>
-      </c>
-      <c r="E18" s="23" t="s">
+      <c r="D18" s="18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="4">
         <v>16</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1295,7 +1303,7 @@
       <c r="C19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="21">
         <v>5</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1304,10 +1312,10 @@
       <c r="G19" s="4">
         <v>17</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1318,7 +1326,7 @@
       <c r="C20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="21">
         <v>13</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -1327,10 +1335,10 @@
       <c r="G20" s="6">
         <v>18</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="17" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1341,7 +1349,7 @@
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="21">
         <v>14</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -1355,7 +1363,7 @@
       <c r="C22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="21">
         <v>15</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -1369,7 +1377,7 @@
       <c r="C23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="22">
         <v>16</v>
       </c>
       <c r="E23" s="7" t="s">

</xml_diff>

<commit_message>
Termine la parte de gestion de perfiles y elimine la opcion de crear patentes
</commit_message>
<xml_diff>
--- a/Gestion de permisos.xlsx
+++ b/Gestion de permisos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\UAI\5- 1er Cuatrimestre 2024\Ingenieria de software\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014B92F5-ACB4-49E1-AFE6-1D58AF060C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF59A54-AD59-4582-9E51-5BDD1967BEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AD3337A-49E2-40EF-8661-305EFD547F10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="30">
   <si>
     <t>ID_PADRE</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>GestionarCatalogos</t>
+  </si>
+  <si>
+    <t>Encargado</t>
+  </si>
+  <si>
+    <t>Cocinero</t>
+  </si>
+  <si>
+    <t>GestionarComanda</t>
   </si>
 </sst>
 </file>
@@ -154,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -401,11 +410,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -457,13 +477,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9C73EA-1742-4FF6-8289-F6FEEBCE1BA8}">
   <dimension ref="B1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,14 +862,14 @@
       <c r="I2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="N2" s="23" t="s">
+      <c r="L2" s="27"/>
+      <c r="N2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="23"/>
+      <c r="O2" s="27"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -866,7 +887,7 @@
       <c r="G3" s="8">
         <v>1</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="26" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -901,7 +922,7 @@
       <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="16" t="s">
@@ -936,7 +957,7 @@
       <c r="G5" s="4">
         <v>3</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="16" t="s">
@@ -1060,7 +1081,7 @@
       <c r="G9" s="4">
         <v>7</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="16" t="s">
@@ -1089,7 +1110,7 @@
       <c r="G10" s="4">
         <v>8</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="24" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="16" t="s">
@@ -1112,7 +1133,7 @@
       <c r="G11" s="4">
         <v>9</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="16" t="s">
@@ -1135,16 +1156,16 @@
       <c r="G12" s="4">
         <v>10</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="23"/>
+      <c r="L12" s="27"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -1162,7 +1183,7 @@
       <c r="G13" s="4">
         <v>11</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="24" t="s">
         <v>13</v>
       </c>
       <c r="I13" s="16" t="s">
@@ -1191,7 +1212,7 @@
       <c r="G14" s="4">
         <v>12</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="24" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="16" t="s">
@@ -1220,7 +1241,7 @@
       <c r="G15" s="4">
         <v>13</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="24" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="16" t="s">
@@ -1243,7 +1264,7 @@
       <c r="G16" s="4">
         <v>14</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="24" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="16" t="s">
@@ -1266,7 +1287,7 @@
       <c r="G17" s="18">
         <v>15</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="19" t="s">
@@ -1289,7 +1310,7 @@
       <c r="G18" s="4">
         <v>16</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="24" t="s">
         <v>24</v>
       </c>
       <c r="I18" s="16" t="s">
@@ -1312,7 +1333,7 @@
       <c r="G19" s="4">
         <v>17</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>26</v>
       </c>
       <c r="I19" s="16" t="s">
@@ -1335,7 +1356,7 @@
       <c r="G20" s="6">
         <v>18</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="23" t="s">
         <v>25</v>
       </c>
       <c r="I20" s="17" t="s">
@@ -1355,6 +1376,15 @@
       <c r="E21" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="G21" s="3">
+        <v>19</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
@@ -1369,6 +1399,15 @@
       <c r="E22" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="G22" s="3">
+        <v>20</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
@@ -1382,6 +1421,15 @@
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
+      </c>
+      <c r="G23" s="3">
+        <v>21</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Las cantidades se suman en el CU de Crear Orden y en el CU verificar pedido se listan todas las estructuras Pedido/producto/ingrediente
</commit_message>
<xml_diff>
--- a/Gestion de permisos.xlsx
+++ b/Gestion de permisos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\UAI\5- 1er Cuatrimestre 2024\Ingenieria de software\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF59A54-AD59-4582-9E51-5BDD1967BEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E326EFC6-5AB9-4CAA-B890-94077DB1A056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AD3337A-49E2-40EF-8661-305EFD547F10}"/>
   </bookViews>
@@ -158,12 +158,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -362,7 +362,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -372,19 +372,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -408,24 +395,13 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -451,40 +427,47 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9C73EA-1742-4FF6-8289-F6FEEBCE1BA8}">
   <dimension ref="B1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,23 +836,23 @@
       <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="N2" s="27" t="s">
+      <c r="L2" s="17"/>
+      <c r="N2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="27"/>
+      <c r="O2" s="17"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -884,13 +867,13 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="24">
         <v>1</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="26" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="4">
@@ -919,13 +902,13 @@
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="19">
         <v>2</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="20" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="4">
@@ -954,13 +937,13 @@
       <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="19">
         <v>3</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="20" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="6">
@@ -989,13 +972,13 @@
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="4">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="16" t="s">
+      <c r="G6" s="19">
+        <v>4</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="20" t="s">
         <v>23</v>
       </c>
       <c r="O6" s="4">
@@ -1018,13 +1001,13 @@
       <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="19">
         <v>5</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="20" t="s">
         <v>23</v>
       </c>
       <c r="N7" s="4">
@@ -1048,13 +1031,13 @@
       <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="19">
         <v>6</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="20" t="s">
         <v>23</v>
       </c>
       <c r="N8" s="4">
@@ -1078,13 +1061,13 @@
       <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="19">
         <v>7</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="20" t="s">
         <v>22</v>
       </c>
       <c r="N9" s="4">
@@ -1107,13 +1090,13 @@
       <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="19">
         <v>8</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1130,13 +1113,13 @@
       <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="19">
         <v>9</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1153,19 +1136,19 @@
       <c r="E12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="19">
         <v>10</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="27" t="s">
+      <c r="I12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="27"/>
+      <c r="L12" s="17"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -1180,13 +1163,13 @@
       <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="19">
         <v>11</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="20" t="s">
         <v>22</v>
       </c>
       <c r="K13" s="4">
@@ -1209,13 +1192,13 @@
       <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="19">
         <v>12</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="20" t="s">
         <v>22</v>
       </c>
       <c r="K14" s="4">
@@ -1238,13 +1221,13 @@
       <c r="E15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="19">
         <v>13</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1261,13 +1244,13 @@
       <c r="E16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="19">
         <v>14</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1284,36 +1267,36 @@
       <c r="E17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="19">
         <v>15</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="18">
+      <c r="B18" s="13">
         <v>6</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="18">
-        <v>4</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="4">
+      <c r="D18" s="13">
+        <v>4</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="19">
         <v>16</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1324,42 +1307,42 @@
       <c r="C19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="15">
         <v>5</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="19">
         <v>17</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>6</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="15">
         <v>13</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="19">
         <v>18</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1370,19 +1353,19 @@
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="15">
         <v>14</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="19">
         <v>19</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="H21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1393,19 +1376,19 @@
       <c r="C22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="15">
         <v>15</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="19">
         <v>20</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1416,19 +1399,19 @@
       <c r="C23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="16">
         <v>16</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="21">
         <v>21</v>
       </c>
-      <c r="H23" s="28" t="s">
+      <c r="H23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="23" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Termine todos los CU, sus DC y DS. Faltan los DER
</commit_message>
<xml_diff>
--- a/Gestion de permisos.xlsx
+++ b/Gestion de permisos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\UAI\5- 1er Cuatrimestre 2024\Ingenieria de software\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E326EFC6-5AB9-4CAA-B890-94077DB1A056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5660FC27-F927-4C52-B4DA-2136571C9BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AD3337A-49E2-40EF-8661-305EFD547F10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AD3337A-49E2-40EF-8661-305EFD547F10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="34">
   <si>
     <t>ID_PADRE</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>GestionarComanda</t>
+  </si>
+  <si>
+    <t>GrupoPrueba</t>
+  </si>
+  <si>
+    <t>VerPedidosRegistrados</t>
+  </si>
+  <si>
+    <t>VerPedidosEnCurso</t>
+  </si>
+  <si>
+    <t>VerPedidosCerrados</t>
   </si>
 </sst>
 </file>
@@ -401,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -437,9 +449,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,13 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -466,6 +468,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -802,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9C73EA-1742-4FF6-8289-F6FEEBCE1BA8}">
-  <dimension ref="B1:P23"/>
+  <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +834,7 @@
     <col min="9" max="9" width="9.140625" style="3"/>
     <col min="12" max="12" width="14.28515625" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -836,23 +851,23 @@
       <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="N2" s="17" t="s">
+      <c r="L2" s="26"/>
+      <c r="N2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="17"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -867,13 +882,13 @@
       <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="20">
         <v>1</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="22" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="4">
@@ -902,13 +917,13 @@
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="18">
         <v>2</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="4">
@@ -937,13 +952,13 @@
       <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="18">
         <v>3</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="6">
@@ -953,10 +968,10 @@
         <v>18</v>
       </c>
       <c r="O5" s="4">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -972,23 +987,23 @@
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="18">
         <v>4</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="O6" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -1001,22 +1016,21 @@
       <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="18">
         <v>5</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="4">
-        <v>3</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="3"/>
+      <c r="O7" s="6">
+        <v>27</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -1031,22 +1045,21 @@
       <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>6</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="4">
+      <c r="O8" s="4">
+        <v>9</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P8" s="3"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -1061,20 +1074,20 @@
       <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="18">
         <v>7</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="4">
+      <c r="I9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="4">
+        <v>10</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
@@ -1090,15 +1103,22 @@
       <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>8</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="I10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="4">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="3"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
@@ -1113,15 +1133,22 @@
       <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="18">
         <v>9</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="I11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="4">
+        <v>11</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="3"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
@@ -1136,19 +1163,25 @@
       <c r="E12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="18">
         <v>10</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="17" t="s">
+      <c r="I12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="17"/>
+      <c r="L12" s="26"/>
+      <c r="N12" s="4">
+        <v>12</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -1163,13 +1196,13 @@
       <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>11</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>22</v>
       </c>
       <c r="K13" s="4">
@@ -1192,13 +1225,13 @@
       <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="18">
         <v>12</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>22</v>
       </c>
       <c r="K14" s="4">
@@ -1221,13 +1254,13 @@
       <c r="E15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>13</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1244,13 +1277,13 @@
       <c r="E16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <v>14</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1267,13 +1300,13 @@
       <c r="E17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="18">
         <v>15</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1290,13 +1323,13 @@
       <c r="E18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="18">
         <v>16</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1313,13 +1346,13 @@
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="18">
         <v>17</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1336,13 +1369,13 @@
       <c r="E20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="18">
         <v>18</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1359,13 +1392,13 @@
       <c r="E21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="18">
         <v>19</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1382,13 +1415,13 @@
       <c r="E22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="18">
         <v>20</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1405,13 +1438,57 @@
       <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="18">
         <v>21</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="23" t="s">
+      <c r="I23" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="8">
+        <v>22</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="4">
+        <v>25</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="4">
+        <v>26</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="6">
+        <v>27</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="28" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadi el cambio de idioma a todas las pantallas y actualice la carpeta
</commit_message>
<xml_diff>
--- a/Gestion de permisos.xlsx
+++ b/Gestion de permisos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\UAI\5- 1er Cuatrimestre 2024\Ingenieria de software\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5660FC27-F927-4C52-B4DA-2136571C9BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326B74CE-07F9-4D77-9BD3-C6A24886A9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AD3337A-49E2-40EF-8661-305EFD547F10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="36">
   <si>
     <t>ID_PADRE</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>VerPedidosCerrados</t>
+  </si>
+  <si>
+    <t>VerPedidosVerificados</t>
+  </si>
+  <si>
+    <t>VerPedidosListos</t>
   </si>
 </sst>
 </file>
@@ -470,9 +476,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,6 +484,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -817,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9C73EA-1742-4FF6-8289-F6FEEBCE1BA8}">
-  <dimension ref="B1:P27"/>
+  <dimension ref="B1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="G2" sqref="G2:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,14 +866,14 @@
       <c r="I2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="N2" s="26" t="s">
+      <c r="L2" s="30"/>
+      <c r="N2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="26"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -1172,10 +1178,10 @@
       <c r="I12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="26"/>
+      <c r="L12" s="30"/>
       <c r="N12" s="4">
         <v>12</v>
       </c>
@@ -1452,10 +1458,10 @@
       <c r="G24" s="8">
         <v>22</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="H24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="30" t="s">
+      <c r="I24" s="29" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1466,7 +1472,7 @@
       <c r="H25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1477,18 +1483,40 @@
       <c r="H26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I26" s="27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="6">
+      <c r="I26" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="8">
         <v>27</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="4">
+        <v>28</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="6">
+        <v>29</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="27" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>